<commit_message>
Add attachements for open bugs
</commit_message>
<xml_diff>
--- a/Car_BugReports/Car_SearchBugs.xlsx
+++ b/Car_BugReports/Car_SearchBugs.xlsx
@@ -327,6 +327,99 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>38101</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>37579</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>4000501</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>5332</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 1"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="17535526" y="2314054"/>
+          <a:ext cx="3962400" cy="1987053"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>66675</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>1803637</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>4591050</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>33907</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Picture 2"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="17564100" y="8118712"/>
+          <a:ext cx="4524375" cy="2268870"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -618,8 +711,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Z8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D1" sqref="D1"/>
+    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="159" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -635,7 +728,7 @@
     <col min="9" max="9" width="15.140625" style="1" customWidth="1"/>
     <col min="10" max="10" width="16.42578125" style="1" customWidth="1"/>
     <col min="11" max="11" width="15.140625" style="1" customWidth="1"/>
-    <col min="12" max="12" width="17.28515625" style="1" customWidth="1"/>
+    <col min="12" max="12" width="95.5703125" style="1" customWidth="1"/>
     <col min="13" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
@@ -924,5 +1017,6 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>